<commit_message>
close issue#7 and update UserDefined Input
</commit_message>
<xml_diff>
--- a/.github/SDPP_MRI_ROI_LookUpTable.xlsx
+++ b/.github/SDPP_MRI_ROI_LookUpTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ABCDStudyNDA\ABCD_DataAnalysis_5.0\SDPP_ABCD_TabulatedData\.github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D05AC52-D1F1-42F8-B2D5-842889BDFB29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E8538B-827B-479B-8767-753F2817949A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASEG" sheetId="3" r:id="rId1"/>
@@ -6087,8 +6087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -6772,7 +6772,7 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -14159,7 +14159,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -14424,13 +14424,15 @@
   <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="24.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.875" customWidth="1"/>
+    <col min="4" max="4" width="47.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -15476,7 +15478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>

</xml_diff>